<commit_message>
feat: added send email with attachments
</commit_message>
<xml_diff>
--- a/Data/Output/DE325476.xlsx
+++ b/Data/Output/DE325476.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reppl\OneDrive\Área de Trabalho\100DaysOfPython\Projeto-CaseNubank-Python\Data\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B0B4BD-169D-48F1-A60A-4222BABEDA11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7378D60-3A51-4235-82E5-2AA86D440907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="2610" windowWidth="23865" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
     <t>DE325476</t>
   </si>
   <si>
-    <t>05/08/2025</t>
+    <t>06/08/2025</t>
   </si>
   <si>
     <t>Mikael Lopes</t>
@@ -101,7 +101,7 @@
     <t>TERMS</t>
   </si>
   <si>
-    <t>Please, Generate Invoices by 04/09/2025</t>
+    <t>Please, Generate Invoices by 05/09/2025</t>
   </si>
 </sst>
 </file>

</xml_diff>